<commit_message>
commit the sop and xml of pxe programing
</commit_message>
<xml_diff>
--- a/Summary Table.xlsx
+++ b/Summary Table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="87">
   <si>
     <t>roaming</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,10 +123,6 @@
   </si>
   <si>
     <t>Test Equipment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Automaiton Testing Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -356,6 +352,14 @@
   </si>
   <si>
     <t>windows 10 32 bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pxe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automaiton Testing Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1765,60 +1769,60 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>26</v>
@@ -1829,34 +1833,34 @@
     </row>
     <row r="3" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
@@ -1864,25 +1868,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>26</v>
@@ -1896,25 +1900,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>26</v>
@@ -1925,28 +1929,28 @@
     </row>
     <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>26</v>
@@ -1957,7 +1961,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>8</v>
@@ -1966,19 +1970,19 @@
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>26</v>
@@ -1989,7 +1993,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>8</v>
@@ -1998,19 +2002,19 @@
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>26</v>
@@ -2021,7 +2025,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>8</v>
@@ -2030,19 +2034,19 @@
         <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>26</v>
@@ -2053,92 +2057,92 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>46</v>
+        <v>84</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>26</v>
@@ -2149,28 +2153,28 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>26</v>
@@ -2181,7 +2185,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>8</v>
@@ -2190,30 +2194,30 @@
         <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>8</v>
@@ -2231,10 +2235,10 @@
         <v>10</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>26</v>
@@ -2245,7 +2249,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>8</v>
@@ -2263,21 +2267,21 @@
         <v>10</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>8</v>
@@ -2286,19 +2290,19 @@
         <v>10</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>26</v>
@@ -2364,57 +2368,57 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>12</v>
@@ -2428,22 +2432,22 @@
     </row>
     <row r="3" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>12</v>
@@ -2460,22 +2464,22 @@
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>12</v>
@@ -2492,25 +2496,25 @@
     </row>
     <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="30" t="s">
         <v>12</v>
@@ -2524,28 +2528,28 @@
     </row>
     <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>26</v>
@@ -2556,28 +2560,28 @@
     </row>
     <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>26</v>
@@ -2588,28 +2592,28 @@
     </row>
     <row r="8" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>26</v>
@@ -2620,28 +2624,28 @@
     </row>
     <row r="9" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>26</v>
@@ -2697,50 +2701,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the Summary Table
</commit_message>
<xml_diff>
--- a/Summary Table.xlsx
+++ b/Summary Table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="89">
   <si>
     <t>roaming</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,10 +115,6 @@
   </si>
   <si>
     <t>程式控制 Linux 環境下中的 Ethernet 存取，已達成待測物執行飛航模式切換。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -197,9 +193,6 @@
   </si>
   <si>
     <t>Processing</t>
-  </si>
-  <si>
-    <t>Processing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -245,10 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>版本自動化更新程式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>漫遊切換自動化測試程式 (ASUS)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -262,10 +251,6 @@
   </si>
   <si>
     <t>解析度測試程式 (Resolution)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS 自動化安裝測試程式 (Legacy)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -306,18 +291,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OS 自動化安裝測試程式 (UEFI for ipv4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS 自動化安裝測試程式 (UEFI for ipv6)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS 自動化安裝測試程式 (Legacy)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GPU 加速測試程式</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,6 +334,41 @@
   <si>
     <t>Automaiton Testing Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本自動化更新程式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(半自動) OS 自動化安裝測試程式 (Legacy)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(半自動) OS 自動化安裝測試程式 (UEFI for ipv4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(半自動) OS 自動化安裝測試程式 (UEFI for ipv6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(全自動) OS 自動化安裝測試程式 (Legacy)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(全自動) OS 自動化安裝測試程式 (UEFI for ipv4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(全自動) OS 自動化安裝測試程式 (UEFI for ipv6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZL Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Processing</t>
   </si>
 </sst>
 </file>
@@ -444,15 +452,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF0070C0"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color rgb="FFFFC000"/>
       <name val="新細明體"/>
       <family val="1"/>
@@ -485,6 +484,15 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -736,22 +744,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1424,8 +1432,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表格1" displayName="表格1" ref="A1:J1048569" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
-  <autoFilter ref="A1:J1048569"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表格1" displayName="表格1" ref="A1:J1048573" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
+  <autoFilter ref="A1:J1048573"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Automaiton Testing Description" dataDxfId="23"/>
     <tableColumn id="2" name="Test Equipment" dataDxfId="22"/>
@@ -1748,20 +1756,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1048569"/>
+  <dimension ref="A1:J1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22" style="15" customWidth="1"/>
-    <col min="3" max="3" width="17.625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="20" style="13" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="44.25" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.75" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.75" style="13" customWidth="1"/>
+    <col min="4" max="4" width="19.375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="19" style="13" customWidth="1"/>
     <col min="6" max="6" width="19.375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="19.375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="12.375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="12.375" style="28" customWidth="1"/>
     <col min="9" max="9" width="10.875" style="13" customWidth="1"/>
     <col min="10" max="10" width="98.125" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="27.875" style="6"/>
@@ -1769,63 +1777,63 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>16</v>
@@ -1833,34 +1841,34 @@
     </row>
     <row r="3" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
@@ -1868,28 +1876,28 @@
         <v>14</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>20</v>
@@ -1900,28 +1908,28 @@
         <v>15</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>20</v>
@@ -1929,31 +1937,31 @@
     </row>
     <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>21</v>
@@ -1961,7 +1969,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>8</v>
@@ -1970,22 +1978,22 @@
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>22</v>
@@ -1993,7 +2001,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>8</v>
@@ -2002,22 +2010,22 @@
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>23</v>
@@ -2025,7 +2033,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>8</v>
@@ -2034,22 +2042,22 @@
         <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>17</v>
@@ -2057,95 +2065,95 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>18</v>
@@ -2153,31 +2161,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>18</v>
@@ -2185,143 +2193,271 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>10</v>
+        <v>78</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>47</v>
+        <v>77</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>10</v>
+        <v>78</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="15" t="s">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="14" t="s">
+      <c r="D21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J21" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="1048569" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1048569" s="16"/>
-      <c r="B1048569" s="17"/>
-      <c r="C1048569" s="18"/>
-      <c r="D1048569" s="18"/>
-      <c r="E1048569" s="18"/>
-      <c r="F1048569" s="18"/>
-      <c r="G1048569" s="28"/>
-      <c r="H1048569" s="28"/>
-      <c r="I1048569" s="18"/>
-      <c r="J1048569" s="19"/>
+    <row r="1048573" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1048573" s="16"/>
+      <c r="B1048573" s="17"/>
+      <c r="C1048573" s="18"/>
+      <c r="D1048573" s="18"/>
+      <c r="E1048573" s="18"/>
+      <c r="F1048573" s="18"/>
+      <c r="G1048573" s="27"/>
+      <c r="H1048573" s="27"/>
+      <c r="I1048573" s="18"/>
+      <c r="J1048573" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2368,63 +2504,63 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>24</v>
@@ -2432,31 +2568,31 @@
     </row>
     <row r="3" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>25</v>
@@ -2464,31 +2600,31 @@
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>24</v>
@@ -2496,31 +2632,31 @@
     </row>
     <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>25</v>
@@ -2528,31 +2664,31 @@
     </row>
     <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>50</v>
+        <v>76</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>24</v>
@@ -2560,31 +2696,31 @@
     </row>
     <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>50</v>
+        <v>76</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>25</v>
@@ -2592,31 +2728,31 @@
     </row>
     <row r="8" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>50</v>
+        <v>76</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>24</v>
@@ -2624,31 +2760,31 @@
     </row>
     <row r="9" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>50</v>
+        <v>76</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>25</v>
@@ -2701,50 +2837,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit the android 8.1 for airplane mode code.
</commit_message>
<xml_diff>
--- a/Summary Table.xlsx
+++ b/Summary Table.xlsx
@@ -165,10 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Automaiton Testing Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AP: Cisco
 PC: DUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -320,10 +316,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Android 8.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>windows 10 32 bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -369,6 +361,14 @@
   </si>
   <si>
     <t>Processing</t>
+  </si>
+  <si>
+    <t>Android 8.1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automaiton Testing Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1777,10 +1777,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>33</v>
@@ -1795,7 +1795,7 @@
         <v>34</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>28</v>
@@ -1809,31 +1809,31 @@
     </row>
     <row r="2" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>16</v>
@@ -1841,34 +1841,34 @@
     </row>
     <row r="3" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
@@ -1876,28 +1876,28 @@
         <v>14</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>20</v>
@@ -1908,28 +1908,28 @@
         <v>15</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>20</v>
@@ -1937,31 +1937,31 @@
     </row>
     <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>21</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>8</v>
@@ -1978,22 +1978,22 @@
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>22</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>8</v>
@@ -2010,22 +2010,22 @@
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>23</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>8</v>
@@ -2042,22 +2042,22 @@
         <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>17</v>
@@ -2065,95 +2065,95 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>18</v>
@@ -2161,31 +2161,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>18</v>
@@ -2193,95 +2193,95 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>45</v>
+        <v>71</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>45</v>
+        <v>71</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>18</v>
@@ -2289,31 +2289,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>45</v>
+        <v>71</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J17" s="14" t="s">
         <v>18</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>8</v>
@@ -2330,30 +2330,30 @@
         <v>13</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>8</v>
@@ -2371,13 +2371,13 @@
         <v>10</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J19" s="14" t="s">
         <v>19</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>8</v>
@@ -2403,21 +2403,21 @@
         <v>10</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>8</v>
@@ -2426,22 +2426,22 @@
         <v>10</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J21" s="14" t="s">
         <v>19</v>
@@ -2504,7 +2504,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2519,7 +2519,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>27</v>
@@ -2536,31 +2536,31 @@
     </row>
     <row r="2" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>24</v>
@@ -2568,22 +2568,22 @@
     </row>
     <row r="3" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>12</v>
@@ -2592,7 +2592,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>25</v>
@@ -2600,22 +2600,22 @@
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>12</v>
@@ -2624,7 +2624,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>24</v>
@@ -2632,31 +2632,31 @@
     </row>
     <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>25</v>
@@ -2664,31 +2664,31 @@
     </row>
     <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>24</v>
@@ -2696,31 +2696,31 @@
     </row>
     <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>48</v>
+        <v>87</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>86</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>25</v>
@@ -2728,31 +2728,31 @@
     </row>
     <row r="8" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>24</v>
@@ -2760,31 +2760,31 @@
     </row>
     <row r="9" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>48</v>
+        <v>87</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>86</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>25</v>
@@ -2837,50 +2837,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>